<commit_message>
tao file excel quan ly viec tao giao dien app gr IT and app chat
</commit_message>
<xml_diff>
--- a/DocumentGrIT.xlsx
+++ b/DocumentGrIT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace\Android\AppMxhIT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C69AE2D1-022D-47C2-8C20-6BBC537AAFAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C00224-A9AC-43A6-BA4B-C8FDFF44D256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{1BD5A4D7-A36F-4724-9CCE-2214274DC5A7}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="Model" sheetId="2" r:id="rId2"/>
     <sheet name="Entity" sheetId="4" r:id="rId3"/>
     <sheet name="Attribute" sheetId="3" r:id="rId4"/>
+    <sheet name="Xử lý" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="206">
   <si>
     <t>Kiểu trả về</t>
   </si>
@@ -50,9 +51,6 @@
     <t>Hoàn thành</t>
   </si>
   <si>
-    <t>Kiểm tra</t>
-  </si>
-  <si>
     <t>Thêm thông tin người dùng</t>
   </si>
   <si>
@@ -80,12 +78,6 @@
     <t>Quyền</t>
   </si>
   <si>
-    <t>quên mật khẩu</t>
-  </si>
-  <si>
-    <t>xác thực email</t>
-  </si>
-  <si>
     <t>Mô tả method</t>
   </si>
   <si>
@@ -107,9 +99,6 @@
     <t>https://localhost:7003/signin</t>
   </si>
   <si>
-    <t>Ok</t>
-  </si>
-  <si>
     <t>Login</t>
   </si>
   <si>
@@ -140,9 +129,6 @@
     <t>ResponseModel</t>
   </si>
   <si>
-    <t>ForgotPasswordModel</t>
-  </si>
-  <si>
     <t>Xác thực thành công</t>
   </si>
   <si>
@@ -161,15 +147,9 @@
     <t>UserInforModel</t>
   </si>
   <si>
-    <t>String linkImage</t>
-  </si>
-  <si>
     <t>String money, String email</t>
   </si>
   <si>
-    <t>String linkimage, String email</t>
-  </si>
-  <si>
     <t>Lấy danh sách biểu cảm theo bài viết</t>
   </si>
   <si>
@@ -191,12 +171,6 @@
     <t>Bài tỏ cảm xúc bài viết</t>
   </si>
   <si>
-    <t>String postId, String id</t>
-  </si>
-  <si>
-    <t>String postId,String userId, int icon</t>
-  </si>
-  <si>
     <t>Model</t>
   </si>
   <si>
@@ -254,9 +228,6 @@
     <t>tin nhắn mô tả trạng thái hiện tại</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>Gender</t>
   </si>
   <si>
@@ -389,9 +360,6 @@
     <t>Expression</t>
   </si>
   <si>
-    <t>Biểu cảm (quy định biểu cảm bên trang atrribute)</t>
-  </si>
-  <si>
     <t>expression</t>
   </si>
   <si>
@@ -567,6 +535,129 @@
   </si>
   <si>
     <t>Hình ảnh bài bán hàng</t>
+  </si>
+  <si>
+    <t>Người kiểm tra</t>
+  </si>
+  <si>
+    <t>Trạng thái kiểm tra</t>
+  </si>
+  <si>
+    <t>Trọng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ok </t>
+  </si>
+  <si>
+    <t>Không cần quan tâm</t>
+  </si>
+  <si>
+    <t>Lấy thông tin người dùng</t>
+  </si>
+  <si>
+    <t>Mã người dùng</t>
+  </si>
+  <si>
+    <t>String email, String userId</t>
+  </si>
+  <si>
+    <t>Hướng dẫn cách xử lý</t>
+  </si>
+  <si>
+    <t>ChangePasswordModel</t>
+  </si>
+  <si>
+    <t>NewPassword</t>
+  </si>
+  <si>
+    <t>OldPassword</t>
+  </si>
+  <si>
+    <t>EditUserImageModel</t>
+  </si>
+  <si>
+    <t>Lấy thông tin người dùng của người khác</t>
+  </si>
+  <si>
+    <t>PostModel</t>
+  </si>
+  <si>
+    <t>Quên mật khẩu</t>
+  </si>
+  <si>
+    <t>Xác thực email</t>
+  </si>
+  <si>
+    <t>CountExpression</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PostIconsModel</t>
+  </si>
+  <si>
+    <t>Số lượng biểu cảm</t>
+  </si>
+  <si>
+    <t>Các biểu cảm có trong bài viết</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>UserImage</t>
+  </si>
+  <si>
+    <t>String postId, String expression</t>
+  </si>
+  <si>
+    <t>Tổng theo loại biểu cảm trong bài viết</t>
+  </si>
+  <si>
+    <t>String count</t>
+  </si>
+  <si>
+    <t>PostCommentsModel</t>
+  </si>
+  <si>
+    <t>mã tài khoản</t>
+  </si>
+  <si>
+    <t>biểu cảm</t>
+  </si>
+  <si>
+    <t>tên người thả</t>
+  </si>
+  <si>
+    <t>avt người thả</t>
+  </si>
+  <si>
+    <t>nội dung comment</t>
+  </si>
+  <si>
+    <t>List Expression</t>
+  </si>
+  <si>
+    <t>Bài tỏ cảm xúc bình luận</t>
+  </si>
+  <si>
+    <t>ExpressionModel</t>
+  </si>
+  <si>
+    <t>thả cho bài viết hay bình luận quy định tại đây</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loại biểu cảm dành cho bài viết hay bình luận </t>
+  </si>
+  <si>
+    <t>1: cmt</t>
+  </si>
+  <si>
+    <t>2: post</t>
+  </si>
+  <si>
+    <t>Quy định biểu cảm tại đây</t>
   </si>
 </sst>
 </file>
@@ -626,7 +717,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -643,10 +734,16 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -656,6 +753,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -972,10 +1084,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4424DE6-DA6F-4401-BF68-1C2796D187E9}">
-  <dimension ref="A1:I107"/>
+  <dimension ref="A1:L110"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C111" sqref="C111"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -987,458 +1099,540 @@
     <col min="5" max="6" width="40.109375" customWidth="1"/>
     <col min="7" max="7" width="52.6640625" customWidth="1"/>
     <col min="8" max="8" width="16.44140625" customWidth="1"/>
+    <col min="9" max="9" width="25.77734375" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" customWidth="1"/>
+    <col min="11" max="11" width="47.88671875" customWidth="1"/>
+    <col min="12" max="12" width="25.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+    </row>
+    <row r="4" spans="1:12" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-    </row>
-    <row r="4" spans="1:9" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="10" t="s">
+      <c r="H4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="L4" s="13" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-    </row>
-    <row r="6" spans="1:9" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>7</v>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+    </row>
+    <row r="6" spans="1:12" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="15" t="s">
+        <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="E6" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="G6" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="H6" s="5">
         <v>1</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>6</v>
+        <v>167</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="15" t="s">
+        <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>32</v>
+      <c r="C7" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>13</v>
+        <v>18</v>
+      </c>
+      <c r="H7" s="5">
+        <v>1</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="K7" s="13"/>
+    </row>
+    <row r="8" spans="1:12" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="15" t="s">
+        <v>180</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>32</v>
+      <c r="D8" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:9" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>14</v>
+      <c r="K8" s="13"/>
+    </row>
+    <row r="9" spans="1:12" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="15" t="s">
+        <v>181</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>34</v>
+      <c r="K9" s="13"/>
+    </row>
+    <row r="10" spans="1:12" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="15" t="s">
+        <v>29</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>28</v>
+      </c>
       <c r="F10" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
-    </row>
-    <row r="11" spans="1:9" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>26</v>
+      <c r="K10" s="13"/>
+    </row>
+    <row r="11" spans="1:12" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="15" t="s">
+        <v>22</v>
       </c>
       <c r="B11" s="3"/>
-      <c r="C11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>32</v>
+      <c r="C11" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
-    </row>
-    <row r="12" spans="1:9" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>29</v>
+      <c r="K11" s="13"/>
+    </row>
+    <row r="12" spans="1:12" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="15" t="s">
+        <v>25</v>
       </c>
       <c r="B12" s="3"/>
-      <c r="C12" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>32</v>
+      <c r="C12" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="1:9" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>27</v>
+      <c r="K12" s="13"/>
+    </row>
+    <row r="13" spans="1:12" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="15" t="s">
+        <v>23</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" s="3" t="s">
+      <c r="K13" s="13"/>
+    </row>
+    <row r="14" spans="1:12" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="1:9" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="1:9" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>31</v>
+      <c r="D14" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="K14" s="9"/>
+    </row>
+    <row r="15" spans="1:12" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="K15" s="9"/>
+    </row>
+    <row r="16" spans="1:12" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="15" t="s">
+        <v>3</v>
       </c>
       <c r="B16" s="3"/>
-      <c r="C16" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>32</v>
+      <c r="C16" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>
     <row r="17" spans="1:9" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
     </row>
     <row r="18" spans="1:9" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="D18" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="3"/>
+      <c r="E18" s="14" t="s">
+        <v>28</v>
+      </c>
       <c r="F18" s="3" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E19" s="2"/>
+    <row r="19" spans="1:9" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>28</v>
+      </c>
       <c r="F19" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-    </row>
-    <row r="20" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-    </row>
-    <row r="21" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D21" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+    </row>
+    <row r="20" spans="1:9" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E21" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
+      <c r="D20" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+    </row>
+    <row r="21" spans="1:9" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
     </row>
     <row r="22" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>49</v>
+      <c r="A22" s="16" t="s">
+        <v>36</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
     <row r="23" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
+      <c r="A23" s="16" t="s">
+        <v>40</v>
+      </c>
       <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
+      <c r="C23" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
     </row>
     <row r="24" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
+      <c r="A24" s="16" t="s">
+        <v>42</v>
+      </c>
       <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
+      <c r="C24" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
     </row>
     <row r="25" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="2"/>
+      <c r="A25" s="16" t="s">
+        <v>198</v>
+      </c>
       <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
+      <c r="C25" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -1608,11 +1802,48 @@
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B107" s="7"/>
+    <row r="41" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+    </row>
+    <row r="42" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+    </row>
+    <row r="43" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+    </row>
+    <row r="110" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B110" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="13">
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="K6:K13"/>
+    <mergeCell ref="L4:L5"/>
     <mergeCell ref="A1:I2"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="A4:A5"/>
@@ -1626,6 +1857,28 @@
   <hyperlinks>
     <hyperlink ref="G6" r:id="rId1" xr:uid="{1E68A5B5-5AC2-4A44-ADB6-93F186264C32}"/>
     <hyperlink ref="G7" r:id="rId2" xr:uid="{4B8147AC-D5F1-4F85-82FD-58FCDC76DE62}"/>
+    <hyperlink ref="C17" location="Model!D20" display="UserInforModel" xr:uid="{AE1AFCE7-0C61-4E60-92A5-74F2931D1DE3}"/>
+    <hyperlink ref="C16" location="Model!D20" display="UserInforModel" xr:uid="{E7EF4921-1599-4796-B7ED-20664551933F}"/>
+    <hyperlink ref="D14" location="Model!D20" display="UserInforModel" xr:uid="{5BE08288-4FE0-4738-B20A-DDAF5925F729}"/>
+    <hyperlink ref="D15" location="Model!D20" display="UserInforModel" xr:uid="{2C2DF530-CE53-4133-A88E-A4AD281BD3A6}"/>
+    <hyperlink ref="D6:D7" location="Model!D13" display="TokenModel" xr:uid="{16BA5014-EB1E-4E73-834C-8D0D1BBCF5E8}"/>
+    <hyperlink ref="D8:D13" location="Model!D17" display="ResponseModel" xr:uid="{E370BBC0-E8BD-4D84-AF89-E53B113243D6}"/>
+    <hyperlink ref="C6" location="Controller!D3" display="SignUpModel" xr:uid="{55809A5B-9889-4EDA-8163-8DABE90C8922}"/>
+    <hyperlink ref="C7" location="Controller!D10" display="SignInModel" xr:uid="{57F464DB-6CF3-41FA-9D04-F58F372F7C9F}"/>
+    <hyperlink ref="C11:C12" location="Model!D10" display="SignInModel" xr:uid="{1B6BC13A-7D13-481F-A6D4-21636D47CAB0}"/>
+    <hyperlink ref="C12" location="Model!D28" display="ChangePasswordModel" xr:uid="{59049D8F-545E-411E-913F-709B2B6E35DF}"/>
+    <hyperlink ref="C18:C19" location="Model!D32" display="EditUserImageModel" xr:uid="{207D5573-9470-4B8B-A923-036D2DAF77C8}"/>
+    <hyperlink ref="D18" location="Model!D17" display="ResponseModel" xr:uid="{EB3DD7CF-6F92-41BE-BAD0-1D6894B63C96}"/>
+    <hyperlink ref="D19" location="Model!D17" display="ResponseModel" xr:uid="{4B31858D-2EC4-43D1-93A4-7A0D47CDAD6A}"/>
+    <hyperlink ref="D16" location="Model!D17" display="ResponseModel" xr:uid="{F6C1DCA5-0F3F-47C8-ADB4-5FFC253778C9}"/>
+    <hyperlink ref="D17" location="Model!D17" display="ResponseModel" xr:uid="{21B664B7-A0D2-4950-A301-7C2BDCFE0E54}"/>
+    <hyperlink ref="D20" location="Controller!D35" display="List PostModel" xr:uid="{3359CD83-58FF-4687-9A33-AA382B2568CC}"/>
+    <hyperlink ref="D22" location="Controller!D41" display="List PostIconsModel" xr:uid="{6F2A6DA1-F8C6-4A86-AE1E-07A81E48BF75}"/>
+    <hyperlink ref="D23" location="Controller!D50" display="List PostCommentsModel" xr:uid="{7709D03C-3737-4EB9-8238-78CE931C0FA8}"/>
+    <hyperlink ref="E6:E24" location="Controller!D17" display="ResponseModel" xr:uid="{50F3C42E-DEAA-4DA4-A221-D9A23B3B0215}"/>
+    <hyperlink ref="D24" location="Controller!D17" display="ResponseModel" xr:uid="{A2902C2B-9DDC-4BE4-9BA7-4D949E37226F}"/>
+    <hyperlink ref="D25" location="Controller!D17" display="ResponseModel" xr:uid="{C65F399A-1DA1-45CA-A874-272913960012}"/>
+    <hyperlink ref="E25" location="Controller!D17" display="ResponseModel" xr:uid="{F681A5B4-0415-438D-A8DE-14F5D3C38F4C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -1634,10 +1887,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C652161-1CAA-485A-B19F-11609CF6A574}">
-  <dimension ref="D2:F24"/>
+  <dimension ref="D2:F416"/>
   <sheetViews>
-    <sheetView topLeftCell="D6" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1649,148 +1902,1446 @@
   <sheetData>
     <row r="2" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="4:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D3" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D4" s="12"/>
+      <c r="E4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D5" s="12"/>
+      <c r="E5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D6" s="12"/>
+      <c r="E6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D7" s="12"/>
+      <c r="E7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D8" s="12"/>
+      <c r="E8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="4:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10" spans="4:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="4:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D11" s="12"/>
+      <c r="E11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="4:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="4:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D13" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" t="s">
         <v>52</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="4:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D14" s="12"/>
+      <c r="E14" t="s">
         <v>53</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="4:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D15" s="12"/>
+      <c r="E15" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="3" spans="4:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F15" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D4" s="10"/>
-      <c r="E4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D5" s="10"/>
-      <c r="E5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D6" s="10"/>
-      <c r="E6" t="s">
+    <row r="16" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D16" s="7"/>
+    </row>
+    <row r="17" spans="4:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D17" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="7" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D7" s="10"/>
-      <c r="E7" t="s">
+      <c r="F17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D18" s="7"/>
+      <c r="E18" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="8" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D8" s="10"/>
-      <c r="E8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="4:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="4:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D10" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="4:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D11" s="10"/>
-      <c r="E11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="4:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D12" s="6"/>
-    </row>
-    <row r="13" spans="4:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D13" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="F18" t="s">
         <v>61</v>
       </c>
-      <c r="F13" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="4:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="10"/>
-      <c r="E14" t="s">
+    </row>
+    <row r="19" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D19" s="7"/>
+    </row>
+    <row r="20" spans="4:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D20" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D21" s="7"/>
+      <c r="E21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D22" s="7"/>
+      <c r="E22" t="s">
         <v>62</v>
       </c>
-      <c r="F14" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="4:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D15" s="10"/>
-      <c r="E15" t="s">
+    </row>
+    <row r="23" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D23" s="7"/>
+      <c r="E23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D24" s="7"/>
+      <c r="E24" t="s">
         <v>63</v>
       </c>
-      <c r="F15" t="s">
+    </row>
+    <row r="25" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D25" s="7"/>
+      <c r="E25" t="s">
+        <v>76</v>
+      </c>
+      <c r="F25" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="26" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D26" s="7"/>
+      <c r="E26" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="4:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D17" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17" t="s">
-        <v>67</v>
-      </c>
-      <c r="F17" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="E18" t="s">
-        <v>68</v>
-      </c>
-      <c r="F18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="4:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D20" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="21" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="E21" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="22" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="E22" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="23" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="E23" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="E24" t="s">
-        <v>74</v>
-      </c>
+    <row r="27" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D27" s="7"/>
+    </row>
+    <row r="28" spans="4:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D28" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="E28" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D29" s="7"/>
+      <c r="E29" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="30" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D30" s="7"/>
+      <c r="E30" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="31" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D31" s="7"/>
+    </row>
+    <row r="32" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D32" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="E32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D33" s="7"/>
+      <c r="E33" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="34" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D34" s="7"/>
+    </row>
+    <row r="35" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D35" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="E35" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D36" s="7"/>
+      <c r="E36" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="37" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D37" s="7"/>
+      <c r="E37" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="38" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D38" s="7"/>
+      <c r="E38" t="s">
+        <v>182</v>
+      </c>
+      <c r="F38" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="39" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D39" s="7"/>
+      <c r="E39" t="s">
+        <v>197</v>
+      </c>
+      <c r="F39" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="40" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D40" s="7"/>
+    </row>
+    <row r="41" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D41" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="E41" t="s">
+        <v>76</v>
+      </c>
+      <c r="F41" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="42" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D42" s="7"/>
+      <c r="E42" t="s">
+        <v>105</v>
+      </c>
+      <c r="F42" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="43" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D43" s="7"/>
+      <c r="E43" t="s">
+        <v>186</v>
+      </c>
+      <c r="F43" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="44" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D44" s="7"/>
+      <c r="E44" t="s">
+        <v>187</v>
+      </c>
+      <c r="F44" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="46" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D46" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="E46" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="47" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D47" s="7"/>
+      <c r="E47" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="48" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D48" s="7"/>
+      <c r="E48" t="s">
+        <v>91</v>
+      </c>
+      <c r="F48" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="49" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D49" s="7"/>
+      <c r="E49" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="50" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D50" s="7"/>
+      <c r="E50" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="51" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D51" s="7"/>
+    </row>
+    <row r="52" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D52" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="E52" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="53" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D53" s="7"/>
+      <c r="E53" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="54" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D54" s="7"/>
+      <c r="E54" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="55" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D55" s="7"/>
+      <c r="E55" t="s">
+        <v>201</v>
+      </c>
+      <c r="F55" s="10" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="56" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D56" s="7"/>
+    </row>
+    <row r="57" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D57" s="7"/>
+    </row>
+    <row r="58" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D58" s="7"/>
+    </row>
+    <row r="59" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D59" s="7"/>
+    </row>
+    <row r="60" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D60" s="7"/>
+    </row>
+    <row r="61" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D61" s="7"/>
+    </row>
+    <row r="62" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D62" s="7"/>
+    </row>
+    <row r="63" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D63" s="7"/>
+    </row>
+    <row r="64" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D64" s="7"/>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D65" s="7"/>
+    </row>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D66" s="7"/>
+    </row>
+    <row r="67" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D67" s="7"/>
+    </row>
+    <row r="68" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D68" s="7"/>
+    </row>
+    <row r="69" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D69" s="7"/>
+    </row>
+    <row r="70" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D70" s="7"/>
+    </row>
+    <row r="71" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D71" s="7"/>
+    </row>
+    <row r="72" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D72" s="7"/>
+    </row>
+    <row r="73" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D73" s="7"/>
+    </row>
+    <row r="74" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D74" s="7"/>
+    </row>
+    <row r="75" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D75" s="7"/>
+    </row>
+    <row r="76" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D76" s="7"/>
+    </row>
+    <row r="77" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D77" s="7"/>
+    </row>
+    <row r="78" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D78" s="7"/>
+    </row>
+    <row r="79" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D79" s="7"/>
+    </row>
+    <row r="80" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D80" s="7"/>
+    </row>
+    <row r="81" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D81" s="7"/>
+    </row>
+    <row r="82" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D82" s="7"/>
+    </row>
+    <row r="83" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D83" s="7"/>
+    </row>
+    <row r="84" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D84" s="7"/>
+    </row>
+    <row r="85" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D85" s="7"/>
+    </row>
+    <row r="86" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D86" s="7"/>
+    </row>
+    <row r="87" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D87" s="7"/>
+    </row>
+    <row r="88" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D88" s="7"/>
+    </row>
+    <row r="89" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D89" s="7"/>
+    </row>
+    <row r="90" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D90" s="7"/>
+    </row>
+    <row r="91" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D91" s="7"/>
+    </row>
+    <row r="92" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D92" s="7"/>
+    </row>
+    <row r="93" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D93" s="7"/>
+    </row>
+    <row r="94" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D94" s="7"/>
+    </row>
+    <row r="95" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D95" s="7"/>
+    </row>
+    <row r="96" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D96" s="7"/>
+    </row>
+    <row r="97" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D97" s="7"/>
+    </row>
+    <row r="98" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D98" s="7"/>
+    </row>
+    <row r="99" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D99" s="7"/>
+    </row>
+    <row r="100" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D100" s="7"/>
+    </row>
+    <row r="101" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D101" s="7"/>
+    </row>
+    <row r="102" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D102" s="7"/>
+    </row>
+    <row r="103" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D103" s="7"/>
+    </row>
+    <row r="104" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D104" s="7"/>
+    </row>
+    <row r="105" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D105" s="7"/>
+    </row>
+    <row r="106" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D106" s="7"/>
+    </row>
+    <row r="107" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D107" s="7"/>
+    </row>
+    <row r="108" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D108" s="7"/>
+    </row>
+    <row r="109" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D109" s="7"/>
+    </row>
+    <row r="110" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D110" s="7"/>
+    </row>
+    <row r="111" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D111" s="7"/>
+    </row>
+    <row r="112" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D112" s="7"/>
+    </row>
+    <row r="113" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D113" s="7"/>
+    </row>
+    <row r="114" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D114" s="7"/>
+    </row>
+    <row r="115" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D115" s="7"/>
+    </row>
+    <row r="116" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D116" s="7"/>
+    </row>
+    <row r="117" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D117" s="7"/>
+    </row>
+    <row r="118" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D118" s="7"/>
+    </row>
+    <row r="119" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D119" s="7"/>
+    </row>
+    <row r="120" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D120" s="7"/>
+    </row>
+    <row r="121" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D121" s="7"/>
+    </row>
+    <row r="122" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D122" s="7"/>
+    </row>
+    <row r="123" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D123" s="7"/>
+    </row>
+    <row r="124" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D124" s="7"/>
+    </row>
+    <row r="125" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D125" s="7"/>
+    </row>
+    <row r="126" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D126" s="7"/>
+    </row>
+    <row r="127" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D127" s="7"/>
+    </row>
+    <row r="128" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D128" s="7"/>
+    </row>
+    <row r="129" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D129" s="7"/>
+    </row>
+    <row r="130" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D130" s="7"/>
+    </row>
+    <row r="131" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D131" s="7"/>
+    </row>
+    <row r="132" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D132" s="7"/>
+    </row>
+    <row r="133" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D133" s="7"/>
+    </row>
+    <row r="134" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D134" s="7"/>
+    </row>
+    <row r="135" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D135" s="7"/>
+    </row>
+    <row r="136" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D136" s="7"/>
+    </row>
+    <row r="137" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D137" s="7"/>
+    </row>
+    <row r="138" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D138" s="7"/>
+    </row>
+    <row r="139" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D139" s="7"/>
+    </row>
+    <row r="140" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D140" s="7"/>
+    </row>
+    <row r="141" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D141" s="7"/>
+    </row>
+    <row r="142" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D142" s="7"/>
+    </row>
+    <row r="143" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D143" s="7"/>
+    </row>
+    <row r="144" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D144" s="7"/>
+    </row>
+    <row r="145" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D145" s="7"/>
+    </row>
+    <row r="146" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D146" s="7"/>
+    </row>
+    <row r="147" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D147" s="7"/>
+    </row>
+    <row r="148" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D148" s="7"/>
+    </row>
+    <row r="149" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D149" s="7"/>
+    </row>
+    <row r="150" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D150" s="7"/>
+    </row>
+    <row r="151" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D151" s="7"/>
+    </row>
+    <row r="152" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D152" s="7"/>
+    </row>
+    <row r="153" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D153" s="7"/>
+    </row>
+    <row r="154" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D154" s="7"/>
+    </row>
+    <row r="155" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D155" s="7"/>
+    </row>
+    <row r="156" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D156" s="7"/>
+    </row>
+    <row r="157" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D157" s="7"/>
+    </row>
+    <row r="158" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D158" s="7"/>
+    </row>
+    <row r="159" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D159" s="7"/>
+    </row>
+    <row r="160" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D160" s="7"/>
+    </row>
+    <row r="161" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D161" s="7"/>
+    </row>
+    <row r="162" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D162" s="7"/>
+    </row>
+    <row r="163" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D163" s="7"/>
+    </row>
+    <row r="164" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D164" s="7"/>
+    </row>
+    <row r="165" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D165" s="7"/>
+    </row>
+    <row r="166" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D166" s="7"/>
+    </row>
+    <row r="167" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D167" s="7"/>
+    </row>
+    <row r="168" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D168" s="7"/>
+    </row>
+    <row r="169" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D169" s="7"/>
+    </row>
+    <row r="170" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D170" s="7"/>
+    </row>
+    <row r="171" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D171" s="7"/>
+    </row>
+    <row r="172" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D172" s="7"/>
+    </row>
+    <row r="173" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D173" s="7"/>
+    </row>
+    <row r="174" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D174" s="7"/>
+    </row>
+    <row r="175" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D175" s="7"/>
+    </row>
+    <row r="176" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D176" s="7"/>
+    </row>
+    <row r="177" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D177" s="7"/>
+    </row>
+    <row r="178" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D178" s="7"/>
+    </row>
+    <row r="179" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D179" s="7"/>
+    </row>
+    <row r="180" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D180" s="7"/>
+    </row>
+    <row r="181" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D181" s="7"/>
+    </row>
+    <row r="182" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D182" s="7"/>
+    </row>
+    <row r="183" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D183" s="7"/>
+    </row>
+    <row r="184" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D184" s="7"/>
+    </row>
+    <row r="185" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D185" s="7"/>
+    </row>
+    <row r="186" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D186" s="7"/>
+    </row>
+    <row r="187" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D187" s="7"/>
+    </row>
+    <row r="188" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D188" s="7"/>
+    </row>
+    <row r="189" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D189" s="7"/>
+    </row>
+    <row r="190" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D190" s="7"/>
+    </row>
+    <row r="191" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D191" s="7"/>
+    </row>
+    <row r="192" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D192" s="7"/>
+    </row>
+    <row r="193" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D193" s="7"/>
+    </row>
+    <row r="194" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D194" s="7"/>
+    </row>
+    <row r="195" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D195" s="7"/>
+    </row>
+    <row r="196" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D196" s="7"/>
+    </row>
+    <row r="197" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D197" s="7"/>
+    </row>
+    <row r="198" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D198" s="7"/>
+    </row>
+    <row r="199" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D199" s="7"/>
+    </row>
+    <row r="200" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D200" s="7"/>
+    </row>
+    <row r="201" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D201" s="7"/>
+    </row>
+    <row r="202" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D202" s="7"/>
+    </row>
+    <row r="203" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D203" s="7"/>
+    </row>
+    <row r="204" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D204" s="7"/>
+    </row>
+    <row r="205" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D205" s="7"/>
+    </row>
+    <row r="206" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D206" s="7"/>
+    </row>
+    <row r="207" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D207" s="7"/>
+    </row>
+    <row r="208" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D208" s="7"/>
+    </row>
+    <row r="209" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D209" s="7"/>
+    </row>
+    <row r="210" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D210" s="7"/>
+    </row>
+    <row r="211" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D211" s="7"/>
+    </row>
+    <row r="212" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D212" s="7"/>
+    </row>
+    <row r="213" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D213" s="7"/>
+    </row>
+    <row r="214" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D214" s="7"/>
+    </row>
+    <row r="215" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D215" s="7"/>
+    </row>
+    <row r="216" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D216" s="7"/>
+    </row>
+    <row r="217" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D217" s="7"/>
+    </row>
+    <row r="218" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D218" s="7"/>
+    </row>
+    <row r="219" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D219" s="7"/>
+    </row>
+    <row r="220" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D220" s="7"/>
+    </row>
+    <row r="221" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D221" s="7"/>
+    </row>
+    <row r="222" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D222" s="7"/>
+    </row>
+    <row r="223" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D223" s="7"/>
+    </row>
+    <row r="224" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D224" s="7"/>
+    </row>
+    <row r="225" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D225" s="7"/>
+    </row>
+    <row r="226" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D226" s="7"/>
+    </row>
+    <row r="227" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D227" s="7"/>
+    </row>
+    <row r="228" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D228" s="7"/>
+    </row>
+    <row r="229" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D229" s="7"/>
+    </row>
+    <row r="230" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D230" s="7"/>
+    </row>
+    <row r="231" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D231" s="7"/>
+    </row>
+    <row r="232" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D232" s="7"/>
+    </row>
+    <row r="233" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D233" s="7"/>
+    </row>
+    <row r="234" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D234" s="7"/>
+    </row>
+    <row r="235" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D235" s="7"/>
+    </row>
+    <row r="236" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D236" s="7"/>
+    </row>
+    <row r="237" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D237" s="7"/>
+    </row>
+    <row r="238" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D238" s="7"/>
+    </row>
+    <row r="239" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D239" s="7"/>
+    </row>
+    <row r="240" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D240" s="7"/>
+    </row>
+    <row r="241" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D241" s="7"/>
+    </row>
+    <row r="242" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D242" s="7"/>
+    </row>
+    <row r="243" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D243" s="7"/>
+    </row>
+    <row r="244" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D244" s="7"/>
+    </row>
+    <row r="245" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D245" s="7"/>
+    </row>
+    <row r="246" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D246" s="7"/>
+    </row>
+    <row r="247" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D247" s="7"/>
+    </row>
+    <row r="248" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D248" s="7"/>
+    </row>
+    <row r="249" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D249" s="7"/>
+    </row>
+    <row r="250" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D250" s="7"/>
+    </row>
+    <row r="251" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D251" s="7"/>
+    </row>
+    <row r="252" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D252" s="7"/>
+    </row>
+    <row r="253" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D253" s="7"/>
+    </row>
+    <row r="254" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D254" s="7"/>
+    </row>
+    <row r="255" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D255" s="7"/>
+    </row>
+    <row r="256" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D256" s="7"/>
+    </row>
+    <row r="257" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D257" s="7"/>
+    </row>
+    <row r="258" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D258" s="7"/>
+    </row>
+    <row r="259" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D259" s="7"/>
+    </row>
+    <row r="260" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D260" s="7"/>
+    </row>
+    <row r="261" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D261" s="7"/>
+    </row>
+    <row r="262" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D262" s="7"/>
+    </row>
+    <row r="263" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D263" s="7"/>
+    </row>
+    <row r="264" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D264" s="7"/>
+    </row>
+    <row r="265" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D265" s="7"/>
+    </row>
+    <row r="266" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D266" s="7"/>
+    </row>
+    <row r="267" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D267" s="7"/>
+    </row>
+    <row r="268" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D268" s="7"/>
+    </row>
+    <row r="269" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D269" s="7"/>
+    </row>
+    <row r="270" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D270" s="7"/>
+    </row>
+    <row r="271" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D271" s="7"/>
+    </row>
+    <row r="272" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D272" s="7"/>
+    </row>
+    <row r="273" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D273" s="7"/>
+    </row>
+    <row r="274" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D274" s="7"/>
+    </row>
+    <row r="275" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D275" s="7"/>
+    </row>
+    <row r="276" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D276" s="7"/>
+    </row>
+    <row r="277" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D277" s="7"/>
+    </row>
+    <row r="278" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D278" s="7"/>
+    </row>
+    <row r="279" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D279" s="7"/>
+    </row>
+    <row r="280" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D280" s="7"/>
+    </row>
+    <row r="281" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D281" s="7"/>
+    </row>
+    <row r="282" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D282" s="7"/>
+    </row>
+    <row r="283" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D283" s="7"/>
+    </row>
+    <row r="284" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D284" s="7"/>
+    </row>
+    <row r="285" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D285" s="7"/>
+    </row>
+    <row r="286" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D286" s="7"/>
+    </row>
+    <row r="287" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D287" s="7"/>
+    </row>
+    <row r="288" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D288" s="7"/>
+    </row>
+    <row r="289" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D289" s="7"/>
+    </row>
+    <row r="290" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D290" s="7"/>
+    </row>
+    <row r="291" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D291" s="7"/>
+    </row>
+    <row r="292" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D292" s="7"/>
+    </row>
+    <row r="293" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D293" s="7"/>
+    </row>
+    <row r="294" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D294" s="7"/>
+    </row>
+    <row r="295" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D295" s="7"/>
+    </row>
+    <row r="296" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D296" s="7"/>
+    </row>
+    <row r="297" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D297" s="7"/>
+    </row>
+    <row r="298" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D298" s="7"/>
+    </row>
+    <row r="299" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D299" s="7"/>
+    </row>
+    <row r="300" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D300" s="7"/>
+    </row>
+    <row r="301" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D301" s="7"/>
+    </row>
+    <row r="302" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D302" s="7"/>
+    </row>
+    <row r="303" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D303" s="7"/>
+    </row>
+    <row r="304" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D304" s="7"/>
+    </row>
+    <row r="305" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D305" s="7"/>
+    </row>
+    <row r="306" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D306" s="7"/>
+    </row>
+    <row r="307" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D307" s="7"/>
+    </row>
+    <row r="308" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D308" s="7"/>
+    </row>
+    <row r="309" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D309" s="7"/>
+    </row>
+    <row r="310" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D310" s="7"/>
+    </row>
+    <row r="311" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D311" s="7"/>
+    </row>
+    <row r="312" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D312" s="7"/>
+    </row>
+    <row r="313" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D313" s="7"/>
+    </row>
+    <row r="314" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D314" s="7"/>
+    </row>
+    <row r="315" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D315" s="7"/>
+    </row>
+    <row r="316" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D316" s="7"/>
+    </row>
+    <row r="317" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D317" s="7"/>
+    </row>
+    <row r="318" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D318" s="7"/>
+    </row>
+    <row r="319" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D319" s="7"/>
+    </row>
+    <row r="320" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D320" s="7"/>
+    </row>
+    <row r="321" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D321" s="7"/>
+    </row>
+    <row r="322" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D322" s="7"/>
+    </row>
+    <row r="323" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D323" s="7"/>
+    </row>
+    <row r="324" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D324" s="7"/>
+    </row>
+    <row r="325" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D325" s="7"/>
+    </row>
+    <row r="326" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D326" s="7"/>
+    </row>
+    <row r="327" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D327" s="7"/>
+    </row>
+    <row r="328" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D328" s="7"/>
+    </row>
+    <row r="329" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D329" s="7"/>
+    </row>
+    <row r="330" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D330" s="7"/>
+    </row>
+    <row r="331" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D331" s="7"/>
+    </row>
+    <row r="332" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D332" s="7"/>
+    </row>
+    <row r="333" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D333" s="7"/>
+    </row>
+    <row r="334" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D334" s="7"/>
+    </row>
+    <row r="335" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D335" s="7"/>
+    </row>
+    <row r="336" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D336" s="7"/>
+    </row>
+    <row r="337" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D337" s="7"/>
+    </row>
+    <row r="338" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D338" s="7"/>
+    </row>
+    <row r="339" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D339" s="7"/>
+    </row>
+    <row r="340" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D340" s="7"/>
+    </row>
+    <row r="341" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D341" s="7"/>
+    </row>
+    <row r="342" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D342" s="7"/>
+    </row>
+    <row r="343" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D343" s="7"/>
+    </row>
+    <row r="344" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D344" s="7"/>
+    </row>
+    <row r="345" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D345" s="7"/>
+    </row>
+    <row r="346" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D346" s="7"/>
+    </row>
+    <row r="347" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D347" s="7"/>
+    </row>
+    <row r="348" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D348" s="7"/>
+    </row>
+    <row r="349" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D349" s="7"/>
+    </row>
+    <row r="350" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D350" s="7"/>
+    </row>
+    <row r="351" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D351" s="7"/>
+    </row>
+    <row r="352" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D352" s="7"/>
+    </row>
+    <row r="353" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D353" s="7"/>
+    </row>
+    <row r="354" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D354" s="7"/>
+    </row>
+    <row r="355" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D355" s="7"/>
+    </row>
+    <row r="356" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D356" s="7"/>
+    </row>
+    <row r="357" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D357" s="7"/>
+    </row>
+    <row r="358" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D358" s="7"/>
+    </row>
+    <row r="359" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D359" s="7"/>
+    </row>
+    <row r="360" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D360" s="7"/>
+    </row>
+    <row r="361" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D361" s="7"/>
+    </row>
+    <row r="362" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D362" s="7"/>
+    </row>
+    <row r="363" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D363" s="7"/>
+    </row>
+    <row r="364" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D364" s="7"/>
+    </row>
+    <row r="365" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D365" s="7"/>
+    </row>
+    <row r="366" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D366" s="7"/>
+    </row>
+    <row r="367" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D367" s="7"/>
+    </row>
+    <row r="368" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D368" s="7"/>
+    </row>
+    <row r="369" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D369" s="7"/>
+    </row>
+    <row r="370" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D370" s="7"/>
+    </row>
+    <row r="371" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D371" s="7"/>
+    </row>
+    <row r="372" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D372" s="7"/>
+    </row>
+    <row r="373" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D373" s="7"/>
+    </row>
+    <row r="374" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D374" s="7"/>
+    </row>
+    <row r="375" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D375" s="7"/>
+    </row>
+    <row r="376" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D376" s="7"/>
+    </row>
+    <row r="377" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D377" s="7"/>
+    </row>
+    <row r="378" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D378" s="7"/>
+    </row>
+    <row r="379" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D379" s="7"/>
+    </row>
+    <row r="380" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D380" s="7"/>
+    </row>
+    <row r="381" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D381" s="7"/>
+    </row>
+    <row r="382" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D382" s="7"/>
+    </row>
+    <row r="383" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D383" s="7"/>
+    </row>
+    <row r="384" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D384" s="7"/>
+    </row>
+    <row r="385" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D385" s="7"/>
+    </row>
+    <row r="386" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D386" s="7"/>
+    </row>
+    <row r="387" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D387" s="7"/>
+    </row>
+    <row r="388" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D388" s="7"/>
+    </row>
+    <row r="389" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D389" s="7"/>
+    </row>
+    <row r="390" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D390" s="7"/>
+    </row>
+    <row r="391" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D391" s="7"/>
+    </row>
+    <row r="392" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D392" s="7"/>
+    </row>
+    <row r="393" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D393" s="7"/>
+    </row>
+    <row r="394" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D394" s="7"/>
+    </row>
+    <row r="395" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D395" s="7"/>
+    </row>
+    <row r="396" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D396" s="7"/>
+    </row>
+    <row r="397" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D397" s="7"/>
+    </row>
+    <row r="398" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D398" s="7"/>
+    </row>
+    <row r="399" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D399" s="7"/>
+    </row>
+    <row r="400" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D400" s="7"/>
+    </row>
+    <row r="401" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D401" s="7"/>
+    </row>
+    <row r="402" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D402" s="7"/>
+    </row>
+    <row r="403" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D403" s="7"/>
+    </row>
+    <row r="404" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D404" s="7"/>
+    </row>
+    <row r="405" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D405" s="7"/>
+    </row>
+    <row r="406" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D406" s="7"/>
+    </row>
+    <row r="407" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D407" s="7"/>
+    </row>
+    <row r="408" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D408" s="7"/>
+    </row>
+    <row r="409" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D409" s="7"/>
+    </row>
+    <row r="410" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D410" s="7"/>
+    </row>
+    <row r="411" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D411" s="7"/>
+    </row>
+    <row r="412" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D412" s="7"/>
+    </row>
+    <row r="413" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D413" s="7"/>
+    </row>
+    <row r="414" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D414" s="7"/>
+    </row>
+    <row r="415" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D415" s="7"/>
+    </row>
+    <row r="416" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D416" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1798,6 +3349,9 @@
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="D13:D15"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="F55" location="Attribute!C12" display="thả cho bài viết hay bình luận quy định tại đây" xr:uid="{E14306BA-F302-4AB3-8927-6A0931545648}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1806,8 +3360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93BFC3DF-28CB-4E11-9643-9F562D8170F9}">
   <dimension ref="C3:H82"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1821,641 +3375,641 @@
   <sheetData>
     <row r="3" spans="3:8" x14ac:dyDescent="0.3">
       <c r="D3" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="E3" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="F3" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="G3" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="H3" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="D4" s="11" t="s">
-        <v>80</v>
+      <c r="D4" s="13" t="s">
+        <v>70</v>
       </c>
       <c r="E4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>161</v>
+        <v>46</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="D5" s="11"/>
+      <c r="D5" s="13"/>
       <c r="E5" t="s">
-        <v>81</v>
-      </c>
-      <c r="H5" s="11"/>
+        <v>71</v>
+      </c>
+      <c r="H5" s="13"/>
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="D6" s="11"/>
+      <c r="D6" s="13"/>
       <c r="E6" t="s">
-        <v>82</v>
-      </c>
-      <c r="H6" s="11"/>
+        <v>72</v>
+      </c>
+      <c r="H6" s="13"/>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
-        <v>171</v>
-      </c>
-      <c r="D7" s="11"/>
+        <v>160</v>
+      </c>
+      <c r="D7" s="13"/>
       <c r="E7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H7" s="13"/>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D8" s="13"/>
+      <c r="E8" t="s">
+        <v>74</v>
+      </c>
+      <c r="H8" s="13"/>
+    </row>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D9" s="13"/>
+      <c r="E9" t="s">
+        <v>53</v>
+      </c>
+      <c r="H9" s="13"/>
+    </row>
+    <row r="10" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D10" s="13"/>
+      <c r="E10" t="s">
+        <v>75</v>
+      </c>
+      <c r="H10" s="13"/>
+    </row>
+    <row r="11" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D11" s="13"/>
+      <c r="E11" t="s">
         <v>83</v>
       </c>
-      <c r="H7" s="11"/>
-    </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="D8" s="11"/>
-      <c r="E8" t="s">
-        <v>84</v>
-      </c>
-      <c r="H8" s="11"/>
-    </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="D9" s="11"/>
-      <c r="E9" t="s">
-        <v>62</v>
-      </c>
-      <c r="H9" s="11"/>
-    </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="D10" s="11"/>
-      <c r="E10" t="s">
+      <c r="F11" t="s">
         <v>85</v>
       </c>
-      <c r="H10" s="11"/>
-    </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="D11" s="11"/>
-      <c r="E11" t="s">
-        <v>93</v>
-      </c>
-      <c r="F11" t="s">
-        <v>95</v>
-      </c>
-      <c r="H11" s="11"/>
+      <c r="H11" s="13"/>
     </row>
     <row r="12" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="H12" s="11"/>
+      <c r="H12" s="13"/>
     </row>
     <row r="13" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="D13" s="11" t="s">
-        <v>87</v>
+      <c r="D13" s="13" t="s">
+        <v>77</v>
       </c>
       <c r="E13" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="F13" t="s">
-        <v>95</v>
-      </c>
-      <c r="H13" s="11"/>
+        <v>85</v>
+      </c>
+      <c r="H13" s="13"/>
     </row>
     <row r="14" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="11"/>
+        <v>11</v>
+      </c>
+      <c r="D14" s="13"/>
       <c r="E14" t="s">
-        <v>89</v>
-      </c>
-      <c r="H14" s="11"/>
+        <v>79</v>
+      </c>
+      <c r="H14" s="13"/>
     </row>
     <row r="15" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="D15" s="11"/>
+      <c r="D15" s="13"/>
       <c r="E15" t="s">
-        <v>90</v>
-      </c>
-      <c r="H15" s="11"/>
+        <v>80</v>
+      </c>
+      <c r="H15" s="13"/>
     </row>
     <row r="16" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="H16" s="11"/>
+      <c r="H16" s="13"/>
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
-        <v>172</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>91</v>
+        <v>161</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>81</v>
       </c>
       <c r="E17" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="F17" t="s">
-        <v>95</v>
-      </c>
-      <c r="H17" s="11"/>
+        <v>85</v>
+      </c>
+      <c r="H17" s="13"/>
     </row>
     <row r="18" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="D18" s="11"/>
+      <c r="D18" s="13"/>
       <c r="E18" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="F18" t="s">
-        <v>95</v>
-      </c>
-      <c r="H18" s="11"/>
+        <v>85</v>
+      </c>
+      <c r="H18" s="13"/>
     </row>
     <row r="19" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="H19" s="11"/>
+      <c r="H19" s="13"/>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="D20" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="E20" t="s">
-        <v>92</v>
-      </c>
-      <c r="H20" s="11"/>
+        <v>82</v>
+      </c>
+      <c r="H20" s="13"/>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.3">
       <c r="E21" t="s">
-        <v>58</v>
-      </c>
-      <c r="H21" s="11"/>
+        <v>49</v>
+      </c>
+      <c r="H21" s="13"/>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.3">
       <c r="E22" t="s">
-        <v>72</v>
-      </c>
-      <c r="H22" s="11"/>
+        <v>62</v>
+      </c>
+      <c r="H22" s="13"/>
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.3">
       <c r="E23" t="s">
-        <v>59</v>
-      </c>
-      <c r="H23" s="11"/>
+        <v>50</v>
+      </c>
+      <c r="H23" s="13"/>
     </row>
     <row r="24" spans="3:8" x14ac:dyDescent="0.3">
       <c r="E24" t="s">
-        <v>73</v>
-      </c>
-      <c r="H24" s="11"/>
+        <v>63</v>
+      </c>
+      <c r="H24" s="13"/>
     </row>
     <row r="25" spans="3:8" x14ac:dyDescent="0.3">
       <c r="E25" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="F25" t="s">
-        <v>95</v>
-      </c>
-      <c r="H25" s="11"/>
+        <v>85</v>
+      </c>
+      <c r="H25" s="13"/>
     </row>
     <row r="26" spans="3:8" x14ac:dyDescent="0.3">
       <c r="E26" t="s">
-        <v>74</v>
-      </c>
-      <c r="H26" s="11"/>
+        <v>64</v>
+      </c>
+      <c r="H26" s="13"/>
     </row>
     <row r="27" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="H27" s="11"/>
+      <c r="H27" s="13"/>
     </row>
     <row r="28" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="D28" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E28" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="F28" t="s">
-        <v>95</v>
-      </c>
-      <c r="H28" s="11"/>
+        <v>85</v>
+      </c>
+      <c r="H28" s="13"/>
     </row>
     <row r="29" spans="3:8" x14ac:dyDescent="0.3">
       <c r="E29" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="G29" t="s">
-        <v>98</v>
-      </c>
-      <c r="H29" s="11"/>
+        <v>88</v>
+      </c>
+      <c r="H29" s="13"/>
     </row>
     <row r="30" spans="3:8" x14ac:dyDescent="0.3">
       <c r="E30" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="G30" t="s">
-        <v>99</v>
-      </c>
-      <c r="H30" s="11"/>
+        <v>89</v>
+      </c>
+      <c r="H30" s="13"/>
     </row>
     <row r="32" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C32" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="D32" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="E32" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="F32" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.3">
       <c r="E33" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="F33" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.3">
       <c r="E34" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="G34" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="35" spans="3:7" x14ac:dyDescent="0.3">
       <c r="E35" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="G35" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C37" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="D37" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="E37" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="F37" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="38" spans="3:7" x14ac:dyDescent="0.3">
       <c r="E38" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="F38" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="G38" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
     </row>
     <row r="39" spans="3:7" x14ac:dyDescent="0.3">
       <c r="E39" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="G39" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
     </row>
     <row r="41" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C41" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="D41" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="E41" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="F41" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="42" spans="3:7" x14ac:dyDescent="0.3">
       <c r="E42" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="F42" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.3">
       <c r="E43" t="s">
-        <v>115</v>
-      </c>
-      <c r="G43" s="8" t="s">
-        <v>116</v>
+        <v>105</v>
+      </c>
+      <c r="G43" s="10" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="45" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C45" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="D45" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="E45" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="F45" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="46" spans="3:7" x14ac:dyDescent="0.3">
       <c r="E46" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="F46" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="47" spans="3:7" x14ac:dyDescent="0.3">
       <c r="E47" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="F47" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="48" spans="3:7" x14ac:dyDescent="0.3">
       <c r="E48" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="G48" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="50" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C50" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="D50" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="E50" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="F50" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="51" spans="3:7" x14ac:dyDescent="0.3">
       <c r="E51" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="F51" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="52" spans="3:7" x14ac:dyDescent="0.3">
       <c r="E52" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="F52" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="53" spans="3:7" x14ac:dyDescent="0.3">
       <c r="E53" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="55" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C55" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="D55" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="E55" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="F55" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="56" spans="3:7" x14ac:dyDescent="0.3">
       <c r="E56" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="F56" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="57" spans="3:7" x14ac:dyDescent="0.3">
       <c r="E57" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="G57" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
     </row>
     <row r="58" spans="3:7" x14ac:dyDescent="0.3">
       <c r="E58" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="G58" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
     </row>
     <row r="60" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C60" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="D60" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="E60" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="F60" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="61" spans="3:7" x14ac:dyDescent="0.3">
       <c r="E61" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="F61" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="G61" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
     </row>
     <row r="62" spans="3:7" x14ac:dyDescent="0.3">
       <c r="E62" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="G62" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
     </row>
     <row r="64" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C64" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="D64" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="E64" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="F64" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="65" spans="3:8" x14ac:dyDescent="0.3">
       <c r="E65" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="F65" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="G65" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
     </row>
     <row r="67" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C67" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="D67" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="E67" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="F67" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="H67" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
     </row>
     <row r="68" spans="3:8" x14ac:dyDescent="0.3">
       <c r="E68" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="F68" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="69" spans="3:8" x14ac:dyDescent="0.3">
       <c r="E69" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
     </row>
     <row r="70" spans="3:8" x14ac:dyDescent="0.3">
       <c r="E70" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="G70" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
     </row>
     <row r="71" spans="3:8" x14ac:dyDescent="0.3">
       <c r="E71" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="G71" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
     </row>
     <row r="72" spans="3:8" x14ac:dyDescent="0.3">
       <c r="E72" t="s">
+        <v>136</v>
+      </c>
+      <c r="G72" t="s">
         <v>147</v>
-      </c>
-      <c r="G72" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="74" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C74" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="D74" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="E74" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="F74" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="75" spans="3:8" x14ac:dyDescent="0.3">
       <c r="E75" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="F75" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="76" spans="3:8" x14ac:dyDescent="0.3">
       <c r="E76" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="G76" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
     </row>
     <row r="77" spans="3:8" x14ac:dyDescent="0.3">
       <c r="E77" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="G77" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
     </row>
     <row r="79" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C79" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="D79" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="E79" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="F79" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="G79" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
     </row>
     <row r="80" spans="3:8" x14ac:dyDescent="0.3">
       <c r="E80" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="F80" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="G80" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
     </row>
     <row r="81" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E81" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="G81" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
     </row>
     <row r="82" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E82" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="G82" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -2466,7 +4020,7 @@
     <mergeCell ref="H4:H30"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G43" location="Attribute!A1" display="Biểu cảm (quy định biểu cảm bên trang atrribute)" xr:uid="{E3722701-4442-42F6-B4D1-61C9BFB98452}"/>
+    <hyperlink ref="G43" location="Attribute!C5" display="Biểu cảm (quy định biểu cảm bên trang atrribute)" xr:uid="{E3722701-4442-42F6-B4D1-61C9BFB98452}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2474,81 +4028,125 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F810536-4F47-4C11-928F-F7B0F0EC963A}">
-  <dimension ref="C4:E10"/>
+  <dimension ref="C4:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C12" sqref="C12:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="21.21875" customWidth="1"/>
     <col min="4" max="4" width="34.33203125" customWidth="1"/>
-    <col min="5" max="5" width="25.109375" customWidth="1"/>
+    <col min="5" max="5" width="52.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="D4" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="E4" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C5" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>117</v>
+      <c r="C5" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>106</v>
       </c>
       <c r="E5" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
       <c r="E6" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
       <c r="E7" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
       <c r="E8" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
       <c r="E9" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
       <c r="E10" t="s">
-        <v>123</v>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C12" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="E12" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="13" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="14" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" t="s">
+        <v>204</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="C5:C10"/>
     <mergeCell ref="D5:D10"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="D12:D14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{043B05EF-2E95-4D07-B4D1-7C3DF8B771F5}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="23.5546875" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix loi file excel doc
</commit_message>
<xml_diff>
--- a/DocumentGrIT.xlsx
+++ b/DocumentGrIT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace\Android\AppMxhIT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C00224-A9AC-43A6-BA4B-C8FDFF44D256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{715769B0-92D8-4B37-B3D8-F891AD2CDB82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{1BD5A4D7-A36F-4724-9CCE-2214274DC5A7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{1BD5A4D7-A36F-4724-9CCE-2214274DC5A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Controller" sheetId="1" r:id="rId1"/>
@@ -745,15 +745,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -768,6 +759,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1086,8 +1086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4424DE6-DA6F-4401-BF68-1C2796D187E9}">
   <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1106,97 +1106,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
     </row>
     <row r="4" spans="1:12" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12" t="s">
+      <c r="E4" s="18"/>
+      <c r="F4" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="18" t="s">
         <v>165</v>
       </c>
-      <c r="J4" s="13" t="s">
+      <c r="J4" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="K4" s="13" t="s">
+      <c r="K4" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="L4" s="13" t="s">
+      <c r="L4" s="16" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
       <c r="D5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
     </row>
     <row r="6" spans="1:12" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="12" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="11" t="s">
         <v>28</v>
       </c>
       <c r="F6" s="3" t="s">
@@ -1214,24 +1214,24 @@
       <c r="J6" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="K6" s="13" t="s">
+      <c r="K6" s="16" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="11" t="s">
         <v>28</v>
       </c>
       <c r="F7" s="3" t="s">
@@ -1249,20 +1249,20 @@
       <c r="J7" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="K7" s="13"/>
+      <c r="K7" s="16"/>
     </row>
     <row r="8" spans="1:12" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="12" t="s">
         <v>180</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="11" t="s">
         <v>28</v>
       </c>
       <c r="F8" s="3" t="s">
@@ -1271,20 +1271,20 @@
       <c r="G8" s="4"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
-      <c r="K8" s="13"/>
+      <c r="K8" s="16"/>
     </row>
     <row r="9" spans="1:12" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="12" t="s">
         <v>181</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="11" t="s">
         <v>28</v>
       </c>
       <c r="F9" s="3" t="s">
@@ -1293,20 +1293,20 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
-      <c r="K9" s="13"/>
+      <c r="K9" s="16"/>
     </row>
     <row r="10" spans="1:12" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="12" t="s">
         <v>29</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="11" t="s">
         <v>28</v>
       </c>
       <c r="F10" s="3" t="s">
@@ -1315,20 +1315,20 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
-      <c r="K10" s="13"/>
+      <c r="K10" s="16"/>
     </row>
     <row r="11" spans="1:12" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="12" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="3"/>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="11" t="s">
         <v>28</v>
       </c>
       <c r="F11" s="3" t="s">
@@ -1337,20 +1337,20 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
-      <c r="K11" s="13"/>
+      <c r="K11" s="16"/>
     </row>
     <row r="12" spans="1:12" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="12" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="3"/>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="11" t="s">
         <v>28</v>
       </c>
       <c r="F12" s="3" t="s">
@@ -1359,20 +1359,20 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
-      <c r="K12" s="13"/>
+      <c r="K12" s="16"/>
     </row>
     <row r="13" spans="1:12" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="12" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="11" t="s">
         <v>28</v>
       </c>
       <c r="F13" s="3" t="s">
@@ -1381,20 +1381,20 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
-      <c r="K13" s="13"/>
+      <c r="K13" s="16"/>
     </row>
     <row r="14" spans="1:12" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="12" t="s">
         <v>170</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="11" t="s">
         <v>28</v>
       </c>
       <c r="F14" s="8" t="s">
@@ -1406,17 +1406,17 @@
       <c r="K14" s="9"/>
     </row>
     <row r="15" spans="1:12" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="12" t="s">
         <v>178</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="11" t="s">
         <v>28</v>
       </c>
       <c r="F15" s="8" t="s">
@@ -1428,17 +1428,17 @@
       <c r="K15" s="9"/>
     </row>
     <row r="16" spans="1:12" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B16" s="3"/>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="11" t="s">
         <v>28</v>
       </c>
       <c r="F16" s="3" t="s">
@@ -1449,17 +1449,17 @@
       <c r="I16" s="3"/>
     </row>
     <row r="17" spans="1:9" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B17" s="3"/>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="11" t="s">
         <v>28</v>
       </c>
       <c r="F17" s="3" t="s">
@@ -1470,17 +1470,17 @@
       <c r="I17" s="3"/>
     </row>
     <row r="18" spans="1:9" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="12" t="s">
         <v>27</v>
       </c>
       <c r="B18" s="3"/>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="11" t="s">
         <v>28</v>
       </c>
       <c r="F18" s="3" t="s">
@@ -1491,17 +1491,17 @@
       <c r="I18" s="3"/>
     </row>
     <row r="19" spans="1:9" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="12" t="s">
         <v>26</v>
       </c>
       <c r="B19" s="3"/>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D19" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="E19" s="11" t="s">
         <v>28</v>
       </c>
       <c r="F19" s="3" t="s">
@@ -1512,17 +1512,17 @@
       <c r="I19" s="3"/>
     </row>
     <row r="20" spans="1:9" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="12" t="s">
         <v>24</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="11" t="s">
         <v>28</v>
       </c>
       <c r="F20" s="8" t="s">
@@ -1533,17 +1533,17 @@
       <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:9" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="12" t="s">
         <v>189</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="D21" s="17" t="s">
+      <c r="D21" s="14" t="s">
         <v>190</v>
       </c>
-      <c r="E21" s="14" t="s">
+      <c r="E21" s="11" t="s">
         <v>28</v>
       </c>
       <c r="F21" s="8" t="s">
@@ -1554,17 +1554,17 @@
       <c r="I21" s="8"/>
     </row>
     <row r="22" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="13" t="s">
         <v>36</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="18" t="s">
+      <c r="D22" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="E22" s="14" t="s">
+      <c r="E22" s="11" t="s">
         <v>28</v>
       </c>
       <c r="F22" s="3" t="s">
@@ -1575,17 +1575,17 @@
       <c r="I22" s="2"/>
     </row>
     <row r="23" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="13" t="s">
         <v>40</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="18" t="s">
+      <c r="D23" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="E23" s="14" t="s">
+      <c r="E23" s="11" t="s">
         <v>28</v>
       </c>
       <c r="F23" s="3" t="s">
@@ -1596,17 +1596,17 @@
       <c r="I23" s="2"/>
     </row>
     <row r="24" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="16" t="s">
+      <c r="A24" s="13" t="s">
         <v>42</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="D24" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="14" t="s">
+      <c r="E24" s="11" t="s">
         <v>28</v>
       </c>
       <c r="F24" s="3" t="s">
@@ -1617,17 +1617,17 @@
       <c r="I24" s="2"/>
     </row>
     <row r="25" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="16" t="s">
+      <c r="A25" s="13" t="s">
         <v>198</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="D25" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E25" s="14" t="s">
+      <c r="E25" s="11" t="s">
         <v>28</v>
       </c>
       <c r="F25" s="8" t="s">
@@ -1863,8 +1863,8 @@
     <hyperlink ref="D15" location="Model!D20" display="UserInforModel" xr:uid="{2C2DF530-CE53-4133-A88E-A4AD281BD3A6}"/>
     <hyperlink ref="D6:D7" location="Model!D13" display="TokenModel" xr:uid="{16BA5014-EB1E-4E73-834C-8D0D1BBCF5E8}"/>
     <hyperlink ref="D8:D13" location="Model!D17" display="ResponseModel" xr:uid="{E370BBC0-E8BD-4D84-AF89-E53B113243D6}"/>
-    <hyperlink ref="C6" location="Controller!D3" display="SignUpModel" xr:uid="{55809A5B-9889-4EDA-8163-8DABE90C8922}"/>
-    <hyperlink ref="C7" location="Controller!D10" display="SignInModel" xr:uid="{57F464DB-6CF3-41FA-9D04-F58F372F7C9F}"/>
+    <hyperlink ref="C6" location="Model!D3" display="SignUpModel" xr:uid="{55809A5B-9889-4EDA-8163-8DABE90C8922}"/>
+    <hyperlink ref="C7" location="Model!D10" display="SignInModel" xr:uid="{57F464DB-6CF3-41FA-9D04-F58F372F7C9F}"/>
     <hyperlink ref="C11:C12" location="Model!D10" display="SignInModel" xr:uid="{1B6BC13A-7D13-481F-A6D4-21636D47CAB0}"/>
     <hyperlink ref="C12" location="Model!D28" display="ChangePasswordModel" xr:uid="{59049D8F-545E-411E-913F-709B2B6E35DF}"/>
     <hyperlink ref="C18:C19" location="Model!D32" display="EditUserImageModel" xr:uid="{207D5573-9470-4B8B-A923-036D2DAF77C8}"/>
@@ -1879,6 +1879,9 @@
     <hyperlink ref="D24" location="Controller!D17" display="ResponseModel" xr:uid="{A2902C2B-9DDC-4BE4-9BA7-4D949E37226F}"/>
     <hyperlink ref="D25" location="Controller!D17" display="ResponseModel" xr:uid="{C65F399A-1DA1-45CA-A874-272913960012}"/>
     <hyperlink ref="E25" location="Controller!D17" display="ResponseModel" xr:uid="{F681A5B4-0415-438D-A8DE-14F5D3C38F4C}"/>
+    <hyperlink ref="D8:D19" location="Model!D17" display="ResponseModel" xr:uid="{5459BDEA-88A9-41EB-B164-30FF71CFDA23}"/>
+    <hyperlink ref="E8:E25" location="Model!D17" display="ResponseModel" xr:uid="{E8C7D93A-C649-4039-8CA4-99FBAE97E723}"/>
+    <hyperlink ref="D24:D25" location="Model!D17" display="ResponseModel" xr:uid="{26318D58-8C7F-44A1-8D38-052926334442}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -1889,8 +1892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C652161-1CAA-485A-B19F-11609CF6A574}">
   <dimension ref="D2:F416"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1912,7 +1915,7 @@
       </c>
     </row>
     <row r="3" spans="4:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="18" t="s">
         <v>14</v>
       </c>
       <c r="E3" t="s">
@@ -1920,31 +1923,31 @@
       </c>
     </row>
     <row r="4" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D4" s="12"/>
+      <c r="D4" s="18"/>
       <c r="E4" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="5" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D5" s="12"/>
+      <c r="D5" s="18"/>
       <c r="E5" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="6" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D6" s="12"/>
+      <c r="D6" s="18"/>
       <c r="E6" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="7" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D7" s="12"/>
+      <c r="D7" s="18"/>
       <c r="E7" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D8" s="12"/>
+      <c r="D8" s="18"/>
       <c r="E8" t="s">
         <v>51</v>
       </c>
@@ -1953,7 +1956,7 @@
       <c r="D9" s="8"/>
     </row>
     <row r="10" spans="4:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="18" t="s">
         <v>20</v>
       </c>
       <c r="E10" t="s">
@@ -1961,7 +1964,7 @@
       </c>
     </row>
     <row r="11" spans="4:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D11" s="12"/>
+      <c r="D11" s="18"/>
       <c r="E11" t="s">
         <v>47</v>
       </c>
@@ -1970,7 +1973,7 @@
       <c r="D12" s="8"/>
     </row>
     <row r="13" spans="4:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="18" t="s">
         <v>16</v>
       </c>
       <c r="E13" t="s">
@@ -1981,7 +1984,7 @@
       </c>
     </row>
     <row r="14" spans="4:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="12"/>
+      <c r="D14" s="18"/>
       <c r="E14" t="s">
         <v>53</v>
       </c>
@@ -1990,7 +1993,7 @@
       </c>
     </row>
     <row r="15" spans="4:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D15" s="12"/>
+      <c r="D15" s="18"/>
       <c r="E15" t="s">
         <v>54</v>
       </c>
@@ -3360,7 +3363,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93BFC3DF-28CB-4E11-9643-9F562D8170F9}">
   <dimension ref="C3:H82"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
@@ -3391,76 +3394,76 @@
       </c>
     </row>
     <row r="4" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="16" t="s">
         <v>70</v>
       </c>
       <c r="E4" t="s">
         <v>46</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="16" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="5" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="D5" s="13"/>
+      <c r="D5" s="16"/>
       <c r="E5" t="s">
         <v>71</v>
       </c>
-      <c r="H5" s="13"/>
+      <c r="H5" s="16"/>
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="D6" s="13"/>
+      <c r="D6" s="16"/>
       <c r="E6" t="s">
         <v>72</v>
       </c>
-      <c r="H6" s="13"/>
+      <c r="H6" s="16"/>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>160</v>
       </c>
-      <c r="D7" s="13"/>
+      <c r="D7" s="16"/>
       <c r="E7" t="s">
         <v>73</v>
       </c>
-      <c r="H7" s="13"/>
+      <c r="H7" s="16"/>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="D8" s="13"/>
+      <c r="D8" s="16"/>
       <c r="E8" t="s">
         <v>74</v>
       </c>
-      <c r="H8" s="13"/>
+      <c r="H8" s="16"/>
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="D9" s="13"/>
+      <c r="D9" s="16"/>
       <c r="E9" t="s">
         <v>53</v>
       </c>
-      <c r="H9" s="13"/>
+      <c r="H9" s="16"/>
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="D10" s="13"/>
+      <c r="D10" s="16"/>
       <c r="E10" t="s">
         <v>75</v>
       </c>
-      <c r="H10" s="13"/>
+      <c r="H10" s="16"/>
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="D11" s="13"/>
+      <c r="D11" s="16"/>
       <c r="E11" t="s">
         <v>83</v>
       </c>
       <c r="F11" t="s">
         <v>85</v>
       </c>
-      <c r="H11" s="13"/>
+      <c r="H11" s="16"/>
     </row>
     <row r="12" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="H12" s="13"/>
+      <c r="H12" s="16"/>
     </row>
     <row r="13" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="16" t="s">
         <v>77</v>
       </c>
       <c r="E13" t="s">
@@ -3469,33 +3472,33 @@
       <c r="F13" t="s">
         <v>85</v>
       </c>
-      <c r="H13" s="13"/>
+      <c r="H13" s="16"/>
     </row>
     <row r="14" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="13"/>
+      <c r="D14" s="16"/>
       <c r="E14" t="s">
         <v>79</v>
       </c>
-      <c r="H14" s="13"/>
+      <c r="H14" s="16"/>
     </row>
     <row r="15" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="D15" s="13"/>
+      <c r="D15" s="16"/>
       <c r="E15" t="s">
         <v>80</v>
       </c>
-      <c r="H15" s="13"/>
+      <c r="H15" s="16"/>
     </row>
     <row r="16" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="H16" s="13"/>
+      <c r="H16" s="16"/>
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
         <v>161</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="16" t="s">
         <v>81</v>
       </c>
       <c r="E17" t="s">
@@ -3504,20 +3507,20 @@
       <c r="F17" t="s">
         <v>85</v>
       </c>
-      <c r="H17" s="13"/>
+      <c r="H17" s="16"/>
     </row>
     <row r="18" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="D18" s="13"/>
+      <c r="D18" s="16"/>
       <c r="E18" t="s">
         <v>78</v>
       </c>
       <c r="F18" t="s">
         <v>85</v>
       </c>
-      <c r="H18" s="13"/>
+      <c r="H18" s="16"/>
     </row>
     <row r="19" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="H19" s="13"/>
+      <c r="H19" s="16"/>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
@@ -3529,31 +3532,31 @@
       <c r="E20" t="s">
         <v>82</v>
       </c>
-      <c r="H20" s="13"/>
+      <c r="H20" s="16"/>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.3">
       <c r="E21" t="s">
         <v>49</v>
       </c>
-      <c r="H21" s="13"/>
+      <c r="H21" s="16"/>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.3">
       <c r="E22" t="s">
         <v>62</v>
       </c>
-      <c r="H22" s="13"/>
+      <c r="H22" s="16"/>
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.3">
       <c r="E23" t="s">
         <v>50</v>
       </c>
-      <c r="H23" s="13"/>
+      <c r="H23" s="16"/>
     </row>
     <row r="24" spans="3:8" x14ac:dyDescent="0.3">
       <c r="E24" t="s">
         <v>63</v>
       </c>
-      <c r="H24" s="13"/>
+      <c r="H24" s="16"/>
     </row>
     <row r="25" spans="3:8" x14ac:dyDescent="0.3">
       <c r="E25" t="s">
@@ -3562,16 +3565,16 @@
       <c r="F25" t="s">
         <v>85</v>
       </c>
-      <c r="H25" s="13"/>
+      <c r="H25" s="16"/>
     </row>
     <row r="26" spans="3:8" x14ac:dyDescent="0.3">
       <c r="E26" t="s">
         <v>64</v>
       </c>
-      <c r="H26" s="13"/>
+      <c r="H26" s="16"/>
     </row>
     <row r="27" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="H27" s="13"/>
+      <c r="H27" s="16"/>
     </row>
     <row r="28" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
@@ -3586,7 +3589,7 @@
       <c r="F28" t="s">
         <v>85</v>
       </c>
-      <c r="H28" s="13"/>
+      <c r="H28" s="16"/>
     </row>
     <row r="29" spans="3:8" x14ac:dyDescent="0.3">
       <c r="E29" t="s">
@@ -3595,7 +3598,7 @@
       <c r="G29" t="s">
         <v>88</v>
       </c>
-      <c r="H29" s="13"/>
+      <c r="H29" s="16"/>
     </row>
     <row r="30" spans="3:8" x14ac:dyDescent="0.3">
       <c r="E30" t="s">
@@ -3604,7 +3607,7 @@
       <c r="G30" t="s">
         <v>89</v>
       </c>
-      <c r="H30" s="13"/>
+      <c r="H30" s="16"/>
     </row>
     <row r="32" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C32" t="s">
@@ -4053,10 +4056,10 @@
       </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="16" t="s">
         <v>106</v>
       </c>
       <c r="E5" t="s">
@@ -4064,45 +4067,45 @@
       </c>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
       <c r="E6" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
       <c r="E7" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
       <c r="E8" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
       <c r="E9" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
       <c r="E10" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="16" t="s">
         <v>201</v>
       </c>
       <c r="E12" t="s">
@@ -4110,15 +4113,15 @@
       </c>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
       <c r="E13" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
       <c r="E14" t="s">
         <v>204</v>
       </c>

</xml_diff>